<commit_message>
changes to data provider function
</commit_message>
<xml_diff>
--- a/src/test/java/Data/TestData.xlsx
+++ b/src/test/java/Data/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -27,39 +27,6 @@
     <t>TC_001_loginandVerify</t>
   </si>
   <si>
-    <t>Value4</t>
-  </si>
-  <si>
-    <t>Value5</t>
-  </si>
-  <si>
-    <t>Value6</t>
-  </si>
-  <si>
-    <t>Value7</t>
-  </si>
-  <si>
-    <t>Value8</t>
-  </si>
-  <si>
-    <t>test2</t>
-  </si>
-  <si>
-    <t>test3</t>
-  </si>
-  <si>
-    <t>test4</t>
-  </si>
-  <si>
-    <t>test5</t>
-  </si>
-  <si>
-    <t>test6</t>
-  </si>
-  <si>
-    <t>test7</t>
-  </si>
-  <si>
     <t>userid</t>
   </si>
   <si>
@@ -85,6 +52,57 @@
   </si>
   <si>
     <t>TC_005_loginandVerify</t>
+  </si>
+  <si>
+    <t>Password01</t>
+  </si>
+  <si>
+    <t>Password02</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MidName </t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>Add2</t>
+  </si>
+  <si>
+    <t>AML admin</t>
+  </si>
+  <si>
+    <t>AML controller</t>
+  </si>
+  <si>
+    <t>UB</t>
+  </si>
+  <si>
+    <t>PRABIN</t>
+  </si>
+  <si>
+    <t>PRAKASH</t>
+  </si>
+  <si>
+    <t>KAUR</t>
+  </si>
+  <si>
+    <t>OSLO</t>
+  </si>
+  <si>
+    <t>EDINBURG</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>London</t>
   </si>
 </sst>
 </file>
@@ -435,7 +453,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -462,7 +480,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
@@ -470,7 +488,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B4" t="b">
         <v>0</v>
@@ -478,7 +496,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B5" t="b">
         <v>0</v>
@@ -486,7 +504,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B6" t="b">
         <v>0</v>
@@ -503,7 +521,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -517,25 +535,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -543,25 +561,25 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -569,51 +587,51 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="H3" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="H4" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>